<commit_message>
Minor change to node timing
</commit_message>
<xml_diff>
--- a/halloween/2024/node_timing.xlsx
+++ b/halloween/2024/node_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\repos\pico-interactive\halloween\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D30B158-5544-4EB2-9609-DBED5ED5E4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57653A-2F8F-4A24-A509-08A1CF717850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DAC233AD-C1FB-4E04-B554-438126B84691}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,9 +825,6 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="C17" s="3"/>
       <c r="F17" s="10"/>
     </row>
@@ -836,7 +833,6 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
       <c r="C18" s="3"/>
       <c r="D18" s="5" t="s">
         <v>31</v>
@@ -849,7 +845,6 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -860,7 +855,6 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
       <c r="C20" s="3"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -871,7 +865,6 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -882,8 +875,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
+      <c r="B22" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="5"/>
@@ -895,6 +888,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -907,6 +901,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="5" t="s">
         <v>32</v>
@@ -921,6 +916,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="F25" s="10" t="s">
         <v>40</v>
@@ -931,6 +927,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="3"/>
       <c r="F26" s="10"/>
     </row>
@@ -938,6 +935,9 @@
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C27" s="3"/>
       <c r="F27" s="10"/>

</xml_diff>